<commit_message>
edit source of SRSSystem
</commit_message>
<xml_diff>
--- a/SRSSystem/SRSSystem/MVCApplication/Data/ZZ/ZZ1031/ZZ1031Data.xlsx
+++ b/SRSSystem/SRSSystem/MVCApplication/Data/ZZ/ZZ1031/ZZ1031Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SRSTraining_OK\SRSSystem\SRSSystem\MVCApplication\Data\ZZ\ZZ1031\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SRSTraining\SRSSystem\SRSSystem\MVCApplication\Data\ZZ\ZZ1031\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -73,17 +73,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>K:東京</t>
-    <rPh sb="2" eb="4">
-      <t>トウキョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>L:東京</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ああああ</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -108,10 +97,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FactoryList</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Remark</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -125,6 +110,18 @@
   </si>
   <si>
     <t>UnitCost</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ListFactory</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>K</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1081,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1098,7 +1095,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1128,31 +1125,31 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
         <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -1205,13 +1202,13 @@
         <v>90000</v>
       </c>
       <c r="Q2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="R2">
         <v>1202</v>
       </c>
       <c r="S2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
@@ -1264,13 +1261,13 @@
         <v>80000</v>
       </c>
       <c r="Q3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="R3">
         <v>1203</v>
       </c>
       <c r="S3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>